<commit_message>
updates to finish MARCC task
</commit_message>
<xml_diff>
--- a/all_motion_feature_data/MissingPercentTable.xlsx
+++ b/all_motion_feature_data/MissingPercentTable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://livejohnshopkins-my.sharepoint.com/personal/sbhatt15_jh_edu/Documents/Shubhayu_Projects/Johns Hopkins University/ICU Motion Study/nims/all_motion_feature_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="22" documentId="11_D045EA1F4C73869CF4AE2FA6EF012D162101B24E" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E40C0474-A566-8F4E-A247-042EFDA4032A}"/>
+  <xr:revisionPtr revIDLastSave="25" documentId="11_D045EA1F4C73869CF4AE2FA6EF012D162101B24E" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E109E0FA-B2AE-C741-A557-B544BE3A3884}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -739,7 +739,7 @@
         <family val="1"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
+      <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -760,6 +760,46 @@
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -918,28 +958,7 @@
         <family val="1"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -961,25 +980,6 @@
       <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -994,20 +994,23 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D025406F-4001-D545-BE90-49944590A3BF}" name="Table1" displayName="Table1" ref="A1:K70" totalsRowShown="0" headerRowDxfId="11" dataDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D025406F-4001-D545-BE90-49944590A3BF}" name="Table1" displayName="Table1" ref="A1:K70" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
   <autoFilter ref="A1:K70" xr:uid="{8AD5409B-DFEE-F343-812B-BF97365F3D7F}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K70">
+    <sortCondition ref="A1:A70"/>
+  </sortState>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{0275474F-D245-4443-B749-B8CDDAD00BA3}" name="Study Patient No." dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{82442017-0F19-9742-84FB-4D3C6A6AB187}" name="Bed" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{6C1883E3-52C7-764E-BB78-1D84AFE2E528}" name="LA" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{2B8DAD2B-DC8F-954A-9085-C4BAA2AC7CEB}" name="LE" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{C91DCBD4-DF10-7C4F-9703-A81C068071BE}" name="LW" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{A27EC3AC-F3EC-F145-83B4-7037696855BC}" name="RA" dataDxfId="3"/>
-    <tableColumn id="7" xr3:uid="{11C136C3-AFB5-024D-BBDF-FB3F7404176E}" name="RE" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{C2171DCF-3869-4546-A2A3-AA0017C78FB5}" name="RW" dataDxfId="0"/>
-    <tableColumn id="9" xr3:uid="{096A4DED-FC04-634B-AA61-F53CD1AB7CE1}" name="Start Timestamp" dataDxfId="1"/>
-    <tableColumn id="10" xr3:uid="{DDEFFD1C-AF2E-AE40-B18C-BDD416F64935}" name="End Timestamp" dataDxfId="10"/>
-    <tableColumn id="11" xr3:uid="{00A66A17-C1D8-E54D-A21B-502724DB72E9}" name="Recording Duration" dataDxfId="9"/>
+    <tableColumn id="1" xr3:uid="{0275474F-D245-4443-B749-B8CDDAD00BA3}" name="Study Patient No." dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{82442017-0F19-9742-84FB-4D3C6A6AB187}" name="Bed" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{6C1883E3-52C7-764E-BB78-1D84AFE2E528}" name="LA" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{2B8DAD2B-DC8F-954A-9085-C4BAA2AC7CEB}" name="LE" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{C91DCBD4-DF10-7C4F-9703-A81C068071BE}" name="LW" dataDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{A27EC3AC-F3EC-F145-83B4-7037696855BC}" name="RA" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{11C136C3-AFB5-024D-BBDF-FB3F7404176E}" name="RE" dataDxfId="4"/>
+    <tableColumn id="8" xr3:uid="{C2171DCF-3869-4546-A2A3-AA0017C78FB5}" name="RW" dataDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{096A4DED-FC04-634B-AA61-F53CD1AB7CE1}" name="Start Timestamp" dataDxfId="2"/>
+    <tableColumn id="10" xr3:uid="{DDEFFD1C-AF2E-AE40-B18C-BDD416F64935}" name="End Timestamp" dataDxfId="1"/>
+    <tableColumn id="11" xr3:uid="{00A66A17-C1D8-E54D-A21B-502724DB72E9}" name="Recording Duration" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1313,7 +1316,7 @@
   <dimension ref="A1:K70"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="200" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>